<commit_message>
Refactor: Remove redundant code and improve structure
- Remove unused CLI parameters (--status-include, --include-overall)
- Remove unnecessary type conversions (int() wrapping pandas results)
- Move main() function to end of file following Python conventions
- Clean up redundant operations for better performance
</commit_message>
<xml_diff>
--- a/out_logs/suite_error_summary.xlsx
+++ b/out_logs/suite_error_summary.xlsx
@@ -17,78 +17,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>BDOR_L8z_Echo</t>
   </si>
   <si>
+    <t>BDOR_BCK_Physical</t>
+  </si>
+  <si>
+    <t>BDOR_L8z_Physical</t>
+  </si>
+  <si>
     <t>ComputerOnly_Tests</t>
   </si>
   <si>
-    <t>BDOR_L8z_Physical</t>
+    <t>BDOR_Standard_Physical</t>
   </si>
   <si>
     <t>BDOR_L3z_Echo</t>
   </si>
   <si>
-    <t>BDOR_BCK_Physical</t>
+    <t>BDOR_L3z_Physical</t>
   </si>
   <si>
     <t>AssertionError: Deploy dialog was not displayed.          09/18/2025 02:28:23 AM      The controller path is set incorrectly.         09/18/2025 02:28:23 AM      Failed to connect with the path 'Ethernet\\\\10.240.158.74\\\\Backplane\\\\0'. Please check path validity and connection.          : expected false to be truthy</t>
   </si>
   <si>
+    <t>\\stexartifacts.file.core.windows.net\regression1\CVB RAIDER\RL-48\job_11783792\CL-36281\CL-38398\TS-139880\TR-20511543\536874621</t>
+  </si>
+  <si>
+    <t>\\stexartifacts.file.core.windows.net\regression1\CVB RAIDER\RL-48\job_11783838\CL-36281\CL-38398\TS-139888\TR-20513063\536880925</t>
+  </si>
+  <si>
     <t>Error: [Project open error dialog] An error is occurring while the system is opening or creating the project.         An \\\Error\\\ dialog is being displayed after complete the base steps to for the project</t>
   </si>
   <si>
+    <t>\\stexartifacts.file.core.windows.net\regression1\CVB RAIDER\RL-48\job_11783833\CL-36281\CL-38398\TS-139887\TR-20512895\536879462</t>
+  </si>
+  <si>
+    <t>STEX execution error</t>
+  </si>
+  <si>
+    <t>\\stexartifacts.file.core.windows.net\regression1\CVB RAIDER\RL-48\job_11783839\CL-36281\CL-38398\TS-139889\TR-20513717\536881233</t>
+  </si>
+  <si>
+    <t>AssertionError: Deploy dialog was not displayed.          09/18/2025 02:27:41 AM      Failed to connect with the path 'Ethernet\\\\10.240.132.161\\\\Backplane\\\\0'. Please check path validity and connection.         09/18/2025 02:27:41 AM      The controller path is set incorrectly.          : expected false to be truthy</t>
+  </si>
+  <si>
+    <t>https://grafana-dev.ftds-dev.rockwellautomation.com/d/XkLVe0Xnk/logs-with-regex-search-2g?&amp;var-LOKI=l-base001&amp;var-query=:(-%7C42287f36-b838-5886-a94b-cc26354e07f7)%5C%5C)&amp;var-stream=stdout&amp;var-namespace=687b63d4-502b-4042-829f-e7b13c92d6a3&amp;var-app=All&amp;var-container=All&amp;var-level=All&amp;from=1758149806919&amp;to=1758150334642</t>
+  </si>
+  <si>
     <t>AssertionError: controller1 is not selected on the deploy grid: expected false to be truthy</t>
   </si>
   <si>
+    <t>Error: [Project open check failure] Timeout opening or creating project e2e_74iwxu65ruf;         the \\\Progress\\\ dialog did not close within expected time</t>
+  </si>
+  <si>
+    <t>https://grafana-dev.ftds-dev.rockwellautomation.com/d/XkLVe0Xnk/logs-with-regex-search-2g?&amp;var-LOKI=l-base001&amp;var-query=:(-%7Cff4d7c31-1e04-5b24-994f-4e5a4bd6890a)%5C%5C)&amp;var-stream=stdout&amp;var-namespace=c3a2582d-60d9-45f1-bf8d-8831224de58c&amp;var-app=All&amp;var-container=All&amp;var-level=All&amp;from=1758152996981&amp;to=1758153308085</t>
+  </si>
+  <si>
     <t>- Error in fixture.after hook -         Run timeout of 2100000ms exceeded.    \]</t>
   </si>
   <si>
+    <t>Test has Timed out after duration of : 68</t>
+  </si>
+  <si>
+    <t>TypeError: Cannot read properties of undefined (reading 'isToolPanelVisible')</t>
+  </si>
+  <si>
     <t>AssertionError: Device is Offline: the given combination of arguments (undefined and string) is invalid for this assertion. You can use an array a map an object a set a string or a weakset instead of a string</t>
   </si>
   <si>
-    <t>AssertionError: Deploy dialog was not displayed.          09/18/2025 02:27:41 AM      Failed to connect with the path 'Ethernet\\\\10.240.132.161\\\\Backplane\\\\0'. Please check path validity and connection.         09/18/2025 02:27:41 AM      The controller path is set incorrectly.          : expected false to be truthy</t>
-  </si>
-  <si>
-    <t>Error: [Project open check failure] Timeout opening or creating project e2e_74iwxu65ruf;         the \\\Progress\\\ dialog did not close within expected time</t>
+    <t>https://grafana-dev.ftds-dev.rockwellautomation.com/d/XkLVe0Xnk/logs-with-regex-search-2g?&amp;var-LOKI=l-base001&amp;var-query=:(-%7C552ad686-a129-53c2-91ca-57c9584b6e30)%5C%5C)&amp;var-stream=stdout&amp;var-namespace=1ed47ba6-277f-4654-93d9-e229951208f7&amp;var-app=All&amp;var-container=All&amp;var-level=All&amp;from=1758152913102&amp;to=1758153386906</t>
+  </si>
+  <si>
+    <t>- Error in fixture.beforeEach hook -         Error: [ERROR] MenuBase: item close_workspace doesn't exist - unable to click</t>
+  </si>
+  <si>
+    <t>Error: No resources for request:   {"resource_type": "Raider-TestStand-PTTIO"; "request_type": "test_stand"; "lab_names_str": "Raider_A"; "accessibility": "Private"; "contains": "Emulate-L3z"}</t>
+  </si>
+  <si>
+    <t>https://grafana-dev.ftds-dev.rockwellautomation.com/d/XkLVe0Xnk/logs-with-regex-search-2g?&amp;var-LOKI=l-base001&amp;var-query=:(-%7C1b9953af-d140-5079-8c16-02cc318af9a7)%5C%5C)&amp;var-stream=stdout&amp;var-namespace=1ed47ba6-277f-4654-93d9-e229951208f7&amp;var-app=All&amp;var-container=All&amp;var-level=All&amp;from=1758153621982&amp;to=1758153885094</t>
+  </si>
+  <si>
+    <t>The specified selector does not match any element in the DOM tree.          &gt; | Selector('.ra-ide-app-shell__main-group__panels__pinned__center-panels .ra-ide-dock-panel__container')            |   .with({ visibilityCheck: true timeout: 500 })            |   .find('.mat-mdc-tab-label-container .static-text-inner')            |   .withExactText('Console')</t>
+  </si>
+  <si>
+    <t>Cannot obtain information about the node because the specified selector does not match any node in the DOM tree.          &gt; | Selector('.cdk-overlay-pane ra-extensible-dialog')            |   .with({ visibilityCheck: true timeout: 500 })            |   .find('.ra-dialog__header')            |   .withAttribute('data-qa-e2e-selector' 'BROWSER_PATH')            |   .parent(0)            |   .find('ra-wwb-entry-wc')            |   .shadowRoot()            |   .find('.mat-dialog-title .dialog-title')</t>
+  </si>
+  <si>
+    <t>AssertionError: RoutineScopedTagRep tag does not exists: expected false to be truthy</t>
+  </si>
+  <si>
+    <t>https://grafana-dev.ftds-dev.rockwellautomation.com/d/XkLVe0Xnk/logs-with-regex-search-2g?&amp;var-LOKI=l-base001&amp;var-query=:(-%7Cb9b8c31a-7a0d-5276-a214-54f5e1ab3933)%5C%5C)&amp;var-stream=stdout&amp;var-namespace=1ed47ba6-277f-4654-93d9-e229951208f7&amp;var-app=All&amp;var-container=All&amp;var-level=All&amp;from=1758154497319&amp;to=1758155843342</t>
   </si>
   <si>
     <t>The specified selector does not match any element in the DOM tree.          &gt; | Selector('.ra-ide-tabs-outlet__context--active .monaco-editor')            |   .with({ visibilityCheck: true timeout: 500 })            |   .find('.view-line')            |   .nth(4)            |   .find('.inlay-hint-editable')            |   .nth(0)            |   .nextSibling()            |   .withText('2')</t>
   </si>
   <si>
-    <t>TypeError: Cannot read properties of undefined (reading 'isToolPanelVisible')</t>
-  </si>
-  <si>
-    <t>- Error in fixture.beforeEach hook -         Error: [ERROR] MenuBase: item close_workspace doesn't exist - unable to click</t>
-  </si>
-  <si>
-    <t>AssertionError: Deploy dialog was not displayed.          09/18/2025 04:40:57 AM      The controller is faulted.          : expected false to be truthy</t>
+    <t>TypeError: Cannot read properties of null (reading 'click')</t>
   </si>
   <si>
     <t>Error: Led stauts is not online  controller:CE1 having issue going online</t>
   </si>
   <si>
-    <t>The specified selector does not match any element in the DOM tree.          &gt; | Selector('.ra-ide-app-shell__main-group__panels__pinned__center-panels .ra-ide-dock-panel__container')            |   .with({ visibilityCheck: true timeout: 500 })            |   .find('.mat-mdc-tab-label-container .static-text-inner')            |   .withExactText('Console')</t>
-  </si>
-  <si>
-    <t>AssertionError: RoutineScopedTagRep tag does not exists: expected false to be truthy</t>
-  </si>
-  <si>
-    <t>Cannot obtain information about the node because the specified selector does not match any node in the DOM tree.          &gt; | Selector('.cdk-overlay-pane ra-extensible-dialog')            |   .with({ visibilityCheck: true timeout: 500 })            |   .find('.ra-dialog__header')            |   .withAttribute('data-qa-e2e-selector' 'BROWSER_PATH')            |   .parent(0)            |   .find('ra-wwb-entry-wc')            |   .shadowRoot()            |   .find('.mat-dialog-title .dialog-title')</t>
-  </si>
-  <si>
-    <t>[1758198434167] There was a backend failure message</t>
-  </si>
-  <si>
-    <t>AssertionError: Deploy dialog was not displayed.          09/18/2025 03:12:38 AM      The controller path is set incorrectly.         09/18/2025 03:12:38 AM      Service method failed          : expected false to be truthy</t>
-  </si>
-  <si>
-    <t>TypeError: Cannot read properties of null (reading 'click')</t>
-  </si>
-  <si>
-    <t>AssertionError: Wrong Device Status displayed :DE3: expected false to be truthy</t>
+    <t>https://grafana-dev.ftds-dev.rockwellautomation.com/d/XkLVe0Xnk/logs-with-regex-search-2g?&amp;var-LOKI=l-base001&amp;var-query=:(-%7C0d1b532a-8617-5f96-9f93-7a2266484c74)%5C%5C)&amp;var-stream=stdout&amp;var-namespace=1ed47ba6-277f-4654-93d9-e229951208f7&amp;var-app=All&amp;var-container=All&amp;var-level=All&amp;from=1758154415197&amp;to=1758156357997</t>
   </si>
   <si>
     <t>Suite</t>
@@ -557,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA7"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -584,49 +617,49 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -637,73 +670,73 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -717,13 +750,13 @@
         <v>326</v>
       </c>
       <c r="D3" s="4">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3" s="4">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="G3" s="4">
         <v>5</v>
@@ -732,10 +765,10 @@
         <v>206</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J3" s="4">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K3" s="4">
         <v>0</v>
@@ -744,10 +777,10 @@
         <v>45</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="N3" s="4">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O3" s="4">
         <v>0</v>
@@ -756,10 +789,10 @@
         <v>31</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="R3" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S3" s="4">
         <v>2</v>
@@ -768,25 +801,25 @@
         <v>16</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="V3" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="W3" s="4">
         <v>0</v>
       </c>
       <c r="X3" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="4">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="Z3" s="4">
         <v>2</v>
       </c>
       <c r="AA3" s="4">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:27">
@@ -794,82 +827,78 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4" s="4">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J4" s="4">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="N4" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3"/>
       <c r="R4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" s="4">
         <v>0</v>
       </c>
       <c r="T4" s="4">
-        <v>1</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="U4" s="3"/>
       <c r="V4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" s="4">
         <v>0</v>
       </c>
       <c r="X4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="4">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -883,46 +912,46 @@
         <v>0</v>
       </c>
       <c r="D5" s="4">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="4">
+      <c r="K5" s="4">
         <v>4</v>
       </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="4">
-        <v>1</v>
-      </c>
-      <c r="K5" s="4">
-        <v>1</v>
-      </c>
       <c r="L5" s="4">
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="N5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O5" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="4">
         <v>0</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="R5" s="4">
         <v>1</v>
@@ -934,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="V5" s="4">
         <v>1</v>
@@ -946,10 +975,10 @@
         <v>0</v>
       </c>
       <c r="Y5" s="4">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="Z5" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="4">
         <v>0</v>
@@ -960,52 +989,52 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4">
+        <v>27</v>
+      </c>
+      <c r="D6" s="4">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
       <c r="K6" s="4">
         <v>0</v>
       </c>
       <c r="L6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="N6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="R6" s="4">
         <v>1</v>
@@ -1016,24 +1045,26 @@
       <c r="T6" s="4">
         <v>1</v>
       </c>
-      <c r="U6" s="3"/>
+      <c r="U6" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="V6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="4">
         <v>0</v>
       </c>
       <c r="X6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="4">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="Z6" s="4">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA6" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1041,29 +1072,31 @@
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="J7" s="4">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K7" s="4">
         <v>0</v>
@@ -1108,6 +1141,172 @@
         <v>0</v>
       </c>
       <c r="AA7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4">
+        <v>1</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="4">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4">
+        <v>1</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V9" s="4">
+        <v>1</v>
+      </c>
+      <c r="W9" s="4">
+        <v>0</v>
+      </c>
+      <c r="X9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="4">
         <v>0</v>
       </c>
     </row>
@@ -1125,6 +1324,14 @@
     <mergeCell ref="U1:X1"/>
     <mergeCell ref="Y1:AA1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1"/>
+    <hyperlink ref="M5" r:id="rId2"/>
+    <hyperlink ref="I7" r:id="rId3"/>
+    <hyperlink ref="M9" r:id="rId4"/>
+    <hyperlink ref="Q9" r:id="rId5"/>
+    <hyperlink ref="U9" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>